<commit_message>
update moving and Insurance Manual_Viavi Solutions_2020.07.01.pdf
</commit_message>
<xml_diff>
--- a/Temp/이사준비-20200605.xlsx
+++ b/Temp/이사준비-20200605.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kan63697\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\04_doc\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D448EBD-32F5-418D-9008-1E4D53D953BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59EB56A-6437-48E5-A5D4-8BE67D22757B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="이사짐센터 견적" sheetId="7" r:id="rId1"/>
@@ -18,13 +18,52 @@
     <sheet name="큰언니네로 갈것" sheetId="5" r:id="rId3"/>
     <sheet name="현대아파트 이사" sheetId="1" r:id="rId4"/>
     <sheet name="자이 입주시" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="MoveToXi" sheetId="3" r:id="rId6"/>
+    <sheet name="OCT" sheetId="9" r:id="rId7"/>
+    <sheet name="NOV" sheetId="10" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'이사짐 센터 견적시 물품'!$C$5:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'이사짐센터 견적'!$B$5:$K$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'자이 입주시'!$A$5:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'현대아파트 이사'!$A$5:$K$84</definedName>
+    <definedName name="DayToStart" localSheetId="7">NOV!$E$1</definedName>
+    <definedName name="DayToStart">OCT!$E$1</definedName>
+    <definedName name="MonthToDisplay" localSheetId="7">NOV!$C$1</definedName>
+    <definedName name="MonthToDisplay" localSheetId="6">OCT!$C$1</definedName>
+    <definedName name="MonthToDisplayNumber" localSheetId="7">MATCH(NOV!MonthToDisplay,NOV!월,0)</definedName>
+    <definedName name="MonthToDisplayNumber" localSheetId="6">MATCH(OCT!MonthToDisplay,월,0)</definedName>
+    <definedName name="ndx" localSheetId="7">ROUNDUP(MATCH(2,1/FREQUENCY(DATE(NOV!표시할연도,NOV!MonthToDisplayNumber,1),NOV!달력))/7,0)</definedName>
+    <definedName name="ndx" localSheetId="6">ROUNDUP(MATCH(2,1/FREQUENCY(DATE(OCT!표시할연도,OCT!MonthToDisplayNumber,1),OCT!달력))/7,0)</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">NOV!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">OCT!$3:$3</definedName>
+    <definedName name="weekdays_reversed" localSheetId="7">{"일요일","토요일","금요일","목요일","수요일","화요일","월요일"}</definedName>
+    <definedName name="weekdays_reversed">{"일요일","토요일","금요일","목요일","수요일","화요일","월요일"}</definedName>
+    <definedName name="날짜눈금" localSheetId="7">NOV!요일+NOV!주*7</definedName>
+    <definedName name="날짜눈금">요일+주*7</definedName>
+    <definedName name="날짜패턴" localSheetId="7">{1,1,2,2,3,3,4,4,5,5,6,6,7}</definedName>
+    <definedName name="날짜패턴">{1,1,2,2,3,3,4,4,5,5,6,6,7}</definedName>
+    <definedName name="달력" localSheetId="7">NOV!날짜눈금+NOV!첫째날짜-WEEKDAY(NOV!첫째날짜)-NOV!요일_옵션</definedName>
+    <definedName name="달력" localSheetId="6">날짜눈금+OCT!첫째날짜-WEEKDAY(OCT!첫째날짜)-요일_옵션</definedName>
+    <definedName name="시작날짜" localSheetId="7">DATE(NOV!표시할연도,NOV!월,1)</definedName>
+    <definedName name="시작날짜" localSheetId="6">DATE(OCT!표시할연도,OCT!월,1)</definedName>
+    <definedName name="요일" localSheetId="7">{0,1,2,3,4,5,6}</definedName>
+    <definedName name="요일">{0,1,2,3,4,5,6}</definedName>
+    <definedName name="요일_옵션" localSheetId="7">MATCH(NOV!DayToStart,NOV!weekdays_reversed,0)-2</definedName>
+    <definedName name="요일_옵션">MATCH(DayToStart,weekdays_reversed,0)-2</definedName>
+    <definedName name="월" localSheetId="7">{"1월","2월","3월","4월","5월","6월","7월","8월","9월","10월","11월","12월"}</definedName>
+    <definedName name="월" localSheetId="7">MATCH(NOV!MonthToDisplay,NOV!월,0)</definedName>
+    <definedName name="월" localSheetId="6">MATCH(OCT!MonthToDisplay,월,0)</definedName>
+    <definedName name="월">{"1월","2월","3월","4월","5월","6월","7월","8월","9월","10월","11월","12월"}</definedName>
+    <definedName name="주" localSheetId="7">{0;1;2;3;4;5;6}</definedName>
+    <definedName name="주">{0;1;2;3;4;5;6}</definedName>
+    <definedName name="첫째날짜" localSheetId="7">DATE(NOV!표시할연도,NOV!월,1)</definedName>
+    <definedName name="첫째날짜" localSheetId="6">DATE(OCT!표시할연도,OCT!월,1)</definedName>
+    <definedName name="평일" localSheetId="7">{"월요일","화요일","수요일","목요일","금요일","토요일","일요일"}</definedName>
+    <definedName name="평일">{"월요일","화요일","수요일","목요일","금요일","토요일","일요일"}</definedName>
+    <definedName name="표시할연도" localSheetId="7">NOV!$B$1</definedName>
+    <definedName name="표시할연도" localSheetId="6">OCT!$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="226">
   <si>
     <t>현대아파트 이사 준비</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -845,13 +884,92 @@
   <si>
     <t>업체4 (믿음익스프레스)</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>schedule</t>
+  </si>
+  <si>
+    <t>10월</t>
+  </si>
+  <si>
+    <t>월요일</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  연도</t>
+  </si>
+  <si>
+    <t>월</t>
+  </si>
+  <si>
+    <t>시작 요일</t>
+  </si>
+  <si>
+    <t>11월</t>
+  </si>
+  <si>
+    <t>탄성코트</t>
+  </si>
+  <si>
+    <t>실외기실-루버창을 수시로 여는 환기가 정답</t>
+  </si>
+  <si>
+    <t>드레스룸 중문설치 - 드레스룸에 냉기가 많을 수 있다고 함</t>
+  </si>
+  <si>
+    <t>줄눈</t>
+  </si>
+  <si>
+    <t>입주청소</t>
+  </si>
+  <si>
+    <t>이사?</t>
+  </si>
+  <si>
+    <t>잔금
+LED 리폼 가능성 타진</t>
+  </si>
+  <si>
+    <t>천장 청소
+아버지 생신</t>
+  </si>
+  <si>
+    <t>탄성코트 전처리</t>
+  </si>
+  <si>
+    <t>탄성코트 전처리 &amp; 환기</t>
+  </si>
+  <si>
+    <t>LED 리폼, LED 간접조명 - 알아보기</t>
+  </si>
+  <si>
+    <t>나노코팅 - 셀프 알아보기</t>
+  </si>
+  <si>
+    <t>환기</t>
+  </si>
+  <si>
+    <t>워시타워
+식기세척기</t>
+  </si>
+  <si>
+    <t>인덕션</t>
+  </si>
+  <si>
+    <t>베이킹, 환기</t>
+  </si>
+  <si>
+    <t>입주청소, 환기</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="aaaa"/>
+    <numFmt numFmtId="165" formatCode="dd"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -899,6 +1017,98 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="32"/>
+      <color theme="4" tint="-0.24994659260841701"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="32"/>
+      <color theme="3"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Malgun Gothic"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -938,7 +1148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -998,13 +1208,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1" tint="0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" applyFill="0" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" applyFill="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1209,6 +1479,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1224,30 +1500,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1263,17 +1539,126 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="7" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="7" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="5" xfId="7" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="6" xfId="8" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="9" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="6" xfId="8" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="6" xfId="8" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="9" applyFont="1" applyFill="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="10">
+    <cellStyle name="날짜 설명" xfId="9" xr:uid="{BF84D2BD-7FFF-419B-83EE-C92AE5859995}"/>
+    <cellStyle name="오른쪽 정렬된 입력 레이블" xfId="6" xr:uid="{BE9D1B82-878C-4CC7-B5E5-BE88E26368D4}"/>
+    <cellStyle name="왼쪽 정렬된 입력 레이블" xfId="5" xr:uid="{45C1AFDB-A987-4B76-A537-319174430331}"/>
+    <cellStyle name="제목 1 2" xfId="1" xr:uid="{1011A572-C383-4780-9A0E-6DC279774EB2}"/>
+    <cellStyle name="제목 2 2" xfId="3" xr:uid="{1E050B4B-FC85-4A0B-A49E-1686A6B2E8AF}"/>
+    <cellStyle name="제목 3 2" xfId="7" xr:uid="{D02B0C82-AE74-42AE-B149-3703B5B798EB}"/>
+    <cellStyle name="제목 4 2" xfId="8" xr:uid="{CFC11C75-DE94-48F9-B149-EC08E91A78B6}"/>
+    <cellStyle name="제목 5" xfId="2" xr:uid="{082425BB-B4A8-4A41-803B-69405D797D4F}"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="4" xr:uid="{DD432FB4-98DC-4BA5-BFAB-A59530CAF70C}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1653,29 +2038,29 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="2:11" s="1" customFormat="1">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="74" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="68" t="s">
+      <c r="D5" s="74"/>
+      <c r="E5" s="70" t="s">
         <v>200</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="69" t="s">
+      <c r="F5" s="70"/>
+      <c r="G5" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="H5" s="69"/>
-      <c r="I5" s="68" t="s">
+      <c r="H5" s="71"/>
+      <c r="I5" s="70" t="s">
         <v>201</v>
       </c>
-      <c r="J5" s="68"/>
+      <c r="J5" s="70"/>
       <c r="K5" s="38"/>
     </row>
     <row r="6" spans="2:11" s="1" customFormat="1">
-      <c r="B6" s="71"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="33" t="s">
         <v>170</v>
       </c>
@@ -2269,10 +2654,10 @@
       <c r="G5" s="38"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="81" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="78" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="34" t="s">
@@ -2285,8 +2670,8 @@
       <c r="G6" s="32"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="73"/>
-      <c r="C7" s="74"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="78"/>
       <c r="D7" s="36" t="s">
         <v>25</v>
       </c>
@@ -2299,8 +2684,8 @@
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="73"/>
-      <c r="C8" s="75" t="s">
+      <c r="B8" s="81"/>
+      <c r="C8" s="82" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="36" t="s">
@@ -2313,8 +2698,8 @@
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="73"/>
-      <c r="C9" s="75"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="34" t="s">
         <v>34</v>
       </c>
@@ -2325,8 +2710,8 @@
       <c r="G9" s="32"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="73"/>
-      <c r="C10" s="74" t="s">
+      <c r="B10" s="81"/>
+      <c r="C10" s="78" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="36" t="s">
@@ -2339,8 +2724,8 @@
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="73"/>
-      <c r="C11" s="74"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="36" t="s">
         <v>114</v>
       </c>
@@ -2351,8 +2736,8 @@
       <c r="G11" s="37"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="73"/>
-      <c r="C12" s="74" t="s">
+      <c r="B12" s="81"/>
+      <c r="C12" s="78" t="s">
         <v>80</v>
       </c>
       <c r="D12" s="36" t="s">
@@ -2365,8 +2750,8 @@
       <c r="G12" s="32"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="73"/>
-      <c r="C13" s="74"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="78"/>
       <c r="D13" s="36" t="s">
         <v>84</v>
       </c>
@@ -2377,8 +2762,8 @@
       <c r="G13" s="37"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="73"/>
-      <c r="C14" s="74"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="36" t="s">
         <v>88</v>
       </c>
@@ -2389,8 +2774,8 @@
       <c r="G14" s="37"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="73"/>
-      <c r="C15" s="74"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="36" t="s">
         <v>115</v>
       </c>
@@ -2417,7 +2802,7 @@
       <c r="G16" s="32"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="81" t="s">
         <v>147</v>
       </c>
       <c r="C17" s="35" t="s">
@@ -2433,7 +2818,7 @@
       <c r="G17" s="32"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="73"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="35" t="s">
         <v>64</v>
       </c>
@@ -2447,10 +2832,10 @@
       <c r="G18" s="32"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="76" t="s">
+      <c r="B19" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="78" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="36" t="s">
@@ -2463,8 +2848,8 @@
       <c r="G19" s="32"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="77"/>
-      <c r="C20" s="74"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="78"/>
       <c r="D20" s="36" t="s">
         <v>17</v>
       </c>
@@ -2475,8 +2860,8 @@
       <c r="G20" s="32"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="77"/>
-      <c r="C21" s="74" t="s">
+      <c r="B21" s="76"/>
+      <c r="C21" s="78" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="36" t="s">
@@ -2489,8 +2874,8 @@
       <c r="G21" s="32"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="77"/>
-      <c r="C22" s="74"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="36" t="s">
         <v>112</v>
       </c>
@@ -2501,7 +2886,7 @@
       <c r="G22" s="37"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="77"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="35" t="s">
         <v>63</v>
       </c>
@@ -2515,7 +2900,7 @@
       <c r="G23" s="32"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="77"/>
+      <c r="B24" s="76"/>
       <c r="C24" s="79" t="s">
         <v>69</v>
       </c>
@@ -2529,7 +2914,7 @@
       <c r="G24" s="32"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="77"/>
+      <c r="B25" s="76"/>
       <c r="C25" s="80"/>
       <c r="D25" s="36" t="s">
         <v>72</v>
@@ -2541,7 +2926,7 @@
       <c r="G25" s="32"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="77"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="35" t="s">
         <v>100</v>
       </c>
@@ -2555,7 +2940,7 @@
       <c r="G26" s="32"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="77"/>
+      <c r="B27" s="76"/>
       <c r="C27" s="79" t="s">
         <v>4</v>
       </c>
@@ -2569,7 +2954,7 @@
       <c r="G27" s="32"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="77"/>
+      <c r="B28" s="76"/>
       <c r="C28" s="80"/>
       <c r="D28" s="36" t="s">
         <v>12</v>
@@ -2581,7 +2966,7 @@
       <c r="G28" s="32"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="77"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="79" t="s">
         <v>81</v>
       </c>
@@ -2595,7 +2980,7 @@
       <c r="G29" s="32"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="78"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="80"/>
       <c r="D30" s="36" t="s">
         <v>83</v>
@@ -3579,18 +3964,18 @@
   </sheetData>
   <autoFilter ref="C5:F5" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="12">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="B19:B30"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3602,7 +3987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:D37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -3641,7 +4026,7 @@
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="84" t="s">
         <v>128</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -3650,35 +4035,35 @@
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="81"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="81"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="81"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="6" t="s">
         <v>112</v>
       </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="81"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="83" t="s">
         <v>127</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -3687,67 +4072,67 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="81"/>
+      <c r="B12" s="83"/>
       <c r="C12" s="26" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="81"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="26" t="s">
         <v>85</v>
       </c>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:4" s="21" customFormat="1">
-      <c r="B14" s="81"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="26" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="81"/>
-      <c r="C15" s="86" t="s">
+      <c r="B15" s="83"/>
+      <c r="C15" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="68" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="81"/>
-      <c r="C16" s="86" t="s">
+      <c r="B16" s="83"/>
+      <c r="C16" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="86" t="s">
+      <c r="D16" s="68" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="81"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="6" t="s">
         <v>83</v>
       </c>
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="81"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="6" t="s">
         <v>120</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="81"/>
+      <c r="B19" s="83"/>
       <c r="C19" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="85" t="s">
         <v>130</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -3756,56 +4141,56 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="84"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="84"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="84"/>
-      <c r="C23" s="86" t="s">
+      <c r="B23" s="86"/>
+      <c r="C23" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="86"/>
+      <c r="D23" s="68"/>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="84"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="84"/>
+      <c r="B25" s="86"/>
       <c r="C25" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="84"/>
+      <c r="B26" s="86"/>
       <c r="C26" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="84"/>
+      <c r="B27" s="86"/>
       <c r="C27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="84"/>
+      <c r="B28" s="86"/>
       <c r="C28" s="6" t="s">
         <v>121</v>
       </c>
@@ -3814,7 +4199,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" s="21" customFormat="1">
-      <c r="B29" s="84"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="6" t="s">
         <v>41</v>
       </c>
@@ -3823,49 +4208,49 @@
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="84"/>
+      <c r="B30" s="86"/>
       <c r="C30" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="84"/>
+      <c r="B31" s="86"/>
       <c r="C31" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="84"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="84"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="6" t="s">
         <v>131</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="84"/>
+      <c r="B34" s="86"/>
       <c r="C34" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="84"/>
+      <c r="B35" s="86"/>
       <c r="C35" s="6" t="s">
         <v>124</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="85"/>
+      <c r="B36" s="87"/>
       <c r="C36" s="6" t="s">
         <v>122</v>
       </c>
@@ -3889,7 +4274,7 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="B86" sqref="B86"/>
@@ -4655,20 +5040,20 @@
       <c r="A42" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="86" t="s">
+      <c r="B42" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="86"/>
-      <c r="D42" s="87"/>
-      <c r="E42" s="87">
-        <v>0</v>
-      </c>
-      <c r="F42" s="87"/>
-      <c r="G42" s="87"/>
-      <c r="H42" s="87"/>
-      <c r="I42" s="87"/>
-      <c r="J42" s="87"/>
-      <c r="K42" s="87"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69">
+        <v>0</v>
+      </c>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="69"/>
+      <c r="K42" s="69"/>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="10" t="s">
@@ -4809,20 +5194,20 @@
       <c r="A50" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="86" t="s">
+      <c r="B50" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="86"/>
-      <c r="D50" s="87"/>
-      <c r="E50" s="87">
-        <v>0</v>
-      </c>
-      <c r="F50" s="87"/>
-      <c r="G50" s="87"/>
-      <c r="H50" s="87"/>
-      <c r="I50" s="87"/>
-      <c r="J50" s="87"/>
-      <c r="K50" s="87"/>
+      <c r="C50" s="68"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69">
+        <v>0</v>
+      </c>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="69"/>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="9" t="s">
@@ -5075,20 +5460,20 @@
       <c r="A64" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="86" t="s">
+      <c r="B64" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="86"/>
-      <c r="D64" s="87">
-        <v>0</v>
-      </c>
-      <c r="E64" s="87"/>
-      <c r="F64" s="87"/>
-      <c r="G64" s="87"/>
-      <c r="H64" s="87"/>
-      <c r="I64" s="87"/>
-      <c r="J64" s="87"/>
-      <c r="K64" s="87"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="69">
+        <v>0</v>
+      </c>
+      <c r="E64" s="69"/>
+      <c r="F64" s="69"/>
+      <c r="G64" s="69"/>
+      <c r="H64" s="69"/>
+      <c r="I64" s="69"/>
+      <c r="J64" s="69"/>
+      <c r="K64" s="69"/>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="10" t="s">
@@ -6068,13 +6453,824 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1F8A40-99C3-4069-BFFD-3A6DF1C722B3}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:H28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="2.5703125" style="91" customWidth="1"/>
+    <col min="2" max="8" width="23.5703125" style="91" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="91"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="45" customHeight="1">
+      <c r="B1" s="88">
+        <f ca="1">YEAR(TODAY())</f>
+        <v>2020</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="89"/>
+      <c r="E1" s="90" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="30" customHeight="1">
+      <c r="B2" s="92" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B3" s="95">
+        <f t="array" aca="1" ref="B3:H3" ca="1">달력</f>
+        <v>44095</v>
+      </c>
+      <c r="C3" s="95">
+        <f ca="1"/>
+        <v>44096</v>
+      </c>
+      <c r="D3" s="95">
+        <f ca="1"/>
+        <v>44097</v>
+      </c>
+      <c r="E3" s="95">
+        <f ca="1"/>
+        <v>44098</v>
+      </c>
+      <c r="F3" s="95">
+        <f ca="1"/>
+        <v>44099</v>
+      </c>
+      <c r="G3" s="96">
+        <f ca="1"/>
+        <v>44100</v>
+      </c>
+      <c r="H3" s="97">
+        <f ca="1"/>
+        <v>44101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="24" customHeight="1">
+      <c r="B4" s="98">
+        <f t="array" aca="1" ref="B4:H4" ca="1">INDEX(달력,ndx+0)</f>
+        <v>44102</v>
+      </c>
+      <c r="C4" s="98">
+        <f ca="1"/>
+        <v>44103</v>
+      </c>
+      <c r="D4" s="98">
+        <f ca="1"/>
+        <v>44104</v>
+      </c>
+      <c r="E4" s="98">
+        <f ca="1"/>
+        <v>44105</v>
+      </c>
+      <c r="F4" s="98">
+        <f ca="1"/>
+        <v>44106</v>
+      </c>
+      <c r="G4" s="100">
+        <f ca="1"/>
+        <v>44107</v>
+      </c>
+      <c r="H4" s="101">
+        <f ca="1"/>
+        <v>44108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="51" customHeight="1">
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+    </row>
+    <row r="6" spans="2:8" ht="24" customHeight="1">
+      <c r="B6" s="98">
+        <f t="array" aca="1" ref="B6:H6" ca="1">INDEX(달력,ndx+1)</f>
+        <v>44109</v>
+      </c>
+      <c r="C6" s="98">
+        <f ca="1"/>
+        <v>44110</v>
+      </c>
+      <c r="D6" s="98">
+        <f ca="1"/>
+        <v>44111</v>
+      </c>
+      <c r="E6" s="98">
+        <f ca="1"/>
+        <v>44112</v>
+      </c>
+      <c r="F6" s="98">
+        <f ca="1"/>
+        <v>44113</v>
+      </c>
+      <c r="G6" s="100">
+        <f ca="1"/>
+        <v>44114</v>
+      </c>
+      <c r="H6" s="101">
+        <f ca="1"/>
+        <v>44115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="51" customHeight="1">
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+    </row>
+    <row r="8" spans="2:8" ht="24" customHeight="1">
+      <c r="B8" s="98">
+        <f t="array" aca="1" ref="B8:H8" ca="1">INDEX(달력,ndx+2)</f>
+        <v>44116</v>
+      </c>
+      <c r="C8" s="98">
+        <f ca="1"/>
+        <v>44117</v>
+      </c>
+      <c r="D8" s="98">
+        <f ca="1"/>
+        <v>44118</v>
+      </c>
+      <c r="E8" s="98">
+        <f ca="1"/>
+        <v>44119</v>
+      </c>
+      <c r="F8" s="98">
+        <f ca="1"/>
+        <v>44120</v>
+      </c>
+      <c r="G8" s="100">
+        <f ca="1"/>
+        <v>44121</v>
+      </c>
+      <c r="H8" s="101">
+        <f ca="1"/>
+        <v>44122</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="51" customHeight="1">
+      <c r="B9" s="99"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+    </row>
+    <row r="10" spans="2:8" ht="24" customHeight="1">
+      <c r="B10" s="98">
+        <f t="array" aca="1" ref="B10:H10" ca="1">INDEX(달력,ndx+3)</f>
+        <v>44123</v>
+      </c>
+      <c r="C10" s="98">
+        <f ca="1"/>
+        <v>44124</v>
+      </c>
+      <c r="D10" s="98">
+        <f ca="1"/>
+        <v>44125</v>
+      </c>
+      <c r="E10" s="98">
+        <f ca="1"/>
+        <v>44126</v>
+      </c>
+      <c r="F10" s="98">
+        <f ca="1"/>
+        <v>44127</v>
+      </c>
+      <c r="G10" s="100">
+        <f ca="1"/>
+        <v>44128</v>
+      </c>
+      <c r="H10" s="101">
+        <f ca="1"/>
+        <v>44129</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="51" customHeight="1">
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+    </row>
+    <row r="12" spans="2:8" ht="24" customHeight="1">
+      <c r="B12" s="98">
+        <f t="array" aca="1" ref="B12:H12" ca="1">INDEX(달력,ndx+4)</f>
+        <v>44130</v>
+      </c>
+      <c r="C12" s="98">
+        <f ca="1"/>
+        <v>44131</v>
+      </c>
+      <c r="D12" s="98">
+        <f ca="1"/>
+        <v>44132</v>
+      </c>
+      <c r="E12" s="98">
+        <f ca="1"/>
+        <v>44133</v>
+      </c>
+      <c r="F12" s="98">
+        <f ca="1"/>
+        <v>44134</v>
+      </c>
+      <c r="G12" s="100">
+        <f ca="1"/>
+        <v>44135</v>
+      </c>
+      <c r="H12" s="98">
+        <f ca="1"/>
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="51" customHeight="1">
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="102" t="s">
+        <v>215</v>
+      </c>
+      <c r="G13" s="99" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" s="99" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="23.25" customHeight="1">
+      <c r="B14" s="98">
+        <f t="array" aca="1" ref="B14:H14" ca="1">INDEX(달력,ndx+5)</f>
+        <v>44137</v>
+      </c>
+      <c r="C14" s="98">
+        <f ca="1"/>
+        <v>44138</v>
+      </c>
+      <c r="D14" s="98">
+        <f ca="1"/>
+        <v>44139</v>
+      </c>
+      <c r="E14" s="98">
+        <f ca="1"/>
+        <v>44140</v>
+      </c>
+      <c r="F14" s="98">
+        <f ca="1"/>
+        <v>44141</v>
+      </c>
+      <c r="G14" s="98">
+        <f ca="1"/>
+        <v>44142</v>
+      </c>
+      <c r="H14" s="98">
+        <f ca="1"/>
+        <v>44143</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="51" customHeight="1">
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="91" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="91" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="91" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="91" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B6:H6">
+    <cfRule type="expression" dxfId="11" priority="6">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:H8">
+    <cfRule type="expression" dxfId="10" priority="5">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B8)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:H10">
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:H12">
+    <cfRule type="expression" dxfId="8" priority="3">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:H14">
+    <cfRule type="expression" dxfId="7" priority="2">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:H4">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 행에는 이 달력의 요일 이름이 표시됩니다. 이 셀에는 주의 시작 요일이 표시됩니다. 시작 요일을 변경하려면 셀 E1에서 새 요일을 입력하거나 선택합니다." sqref="B3" xr:uid="{DD5CA88F-A0C5-41AC-A8BF-9455295DC03F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에는 바로 위의 머리글인 3행에 표시된 요일에 해당하는 시작 날짜가 표시됩니다. 이 셀의 숫자가 1이 아닌 경우 해당 날짜는 이전 달의 날짜가 됩니다. 4, 6, 8, 10, 12, 14행에 각 요일에 해당하는 날짜가 표시됩니다." sqref="B4" xr:uid="{6D35853F-30EA-495A-BC78-CDD26B74986A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이번 달이 12행이나 14행에서 끝나는 경우 12행이나 14행에 다음 달의 날짜가 표시될 수 있습니다." sqref="B12" xr:uid="{89EE7BBE-E46B-45F1-8E1B-C7BB4077BCD2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에 일일 메모를 입력합니다. 5, 7, 9, 11, 13, 15행에는 일별 메모를 입력할 수 있는 셀이 있습니다." sqref="B5" xr:uid="{FD350E77-406C-42B5-8EE0-FA755621C273}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="달력의 연도를 입력합니다." sqref="B1" xr:uid="{9867FC1F-1AC9-4975-ADC9-9DF4863D68E9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 달력은 연도나 월에 관계없이 월이 하나인 달력입니다. C1에서 월을 선택하고 B1에 연도를 입력합니다. 달력의 시작 요일을 E1에서 선택합니다. 5, 7, 9, 11, 13, 15 행에 일일 메모를 입력합니다." sqref="A1" xr:uid="{009356E7-E06F-4B56-AA03-B0B3A812D581}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 월 이름만 이 일정에 적용됩니다. 월 이름을 직접 입력하거나 목록에서 하나를 선택합니다. 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 월을 선택합니다. 월 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 월을 선택하고 ENTER 키를 누릅니다." sqref="C1:D1" xr:uid="{6801CFA1-A028-4615-B440-AB6E0ECF44B9}">
+      <formula1>"1월,2월,3월,4월,5월,6월,7월,8월,9월,10월,11월,12월"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 요일 이름만 이 일정에 적용됩니다. 다시 시도를 선택하고 요일 이름을 직접 입력하거나 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 주 시작 요일을 선택합니다. 요일 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 요일을 선택하고 ENTER 키를 누릅니다." sqref="E1" xr:uid="{D6B12E96-3D93-452B-AF1C-7A9E49BED069}">
+      <formula1>"월요일,화요일,수요일,목요일,금요일,토요일,일요일"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.45" right="0.45" top="0.4" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="87" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1">
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D912176-DD42-45EE-A5A6-3E9852D24924}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:H15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="2.5703125" style="91" customWidth="1"/>
+    <col min="2" max="8" width="23.5703125" style="91" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="91"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="45" customHeight="1">
+      <c r="B1" s="88">
+        <f ca="1">YEAR(TODAY())</f>
+        <v>2020</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="89"/>
+      <c r="E1" s="90" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="30" customHeight="1">
+      <c r="B2" s="92" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B3" s="95">
+        <f t="array" aca="1" ref="B3:H3" ca="1">달력</f>
+        <v>44130</v>
+      </c>
+      <c r="C3" s="95">
+        <f ca="1"/>
+        <v>44131</v>
+      </c>
+      <c r="D3" s="95">
+        <f ca="1"/>
+        <v>44132</v>
+      </c>
+      <c r="E3" s="95">
+        <f ca="1"/>
+        <v>44133</v>
+      </c>
+      <c r="F3" s="95">
+        <f ca="1"/>
+        <v>44134</v>
+      </c>
+      <c r="G3" s="95">
+        <f ca="1"/>
+        <v>44135</v>
+      </c>
+      <c r="H3" s="95">
+        <f ca="1"/>
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="24" customHeight="1">
+      <c r="B4" s="98">
+        <f t="array" aca="1" ref="B4:H4" ca="1">INDEX(달력,ndx+0)</f>
+        <v>44130</v>
+      </c>
+      <c r="C4" s="98">
+        <f ca="1"/>
+        <v>44131</v>
+      </c>
+      <c r="D4" s="98">
+        <f ca="1"/>
+        <v>44132</v>
+      </c>
+      <c r="E4" s="98">
+        <f ca="1"/>
+        <v>44133</v>
+      </c>
+      <c r="F4" s="98">
+        <f ca="1"/>
+        <v>44134</v>
+      </c>
+      <c r="G4" s="98">
+        <f ca="1"/>
+        <v>44135</v>
+      </c>
+      <c r="H4" s="101">
+        <f ca="1"/>
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="51" customHeight="1">
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="24" customHeight="1">
+      <c r="B6" s="98">
+        <f t="array" aca="1" ref="B6:H6" ca="1">INDEX(달력,ndx+1)</f>
+        <v>44137</v>
+      </c>
+      <c r="C6" s="98">
+        <f ca="1"/>
+        <v>44138</v>
+      </c>
+      <c r="D6" s="98">
+        <f ca="1"/>
+        <v>44139</v>
+      </c>
+      <c r="E6" s="98">
+        <f ca="1"/>
+        <v>44140</v>
+      </c>
+      <c r="F6" s="98">
+        <f ca="1"/>
+        <v>44141</v>
+      </c>
+      <c r="G6" s="100">
+        <f ca="1"/>
+        <v>44142</v>
+      </c>
+      <c r="H6" s="101">
+        <f ca="1"/>
+        <v>44143</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="51" customHeight="1">
+      <c r="B7" s="102" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="99" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="102" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="99" t="s">
+        <v>224</v>
+      </c>
+      <c r="F7" s="99" t="s">
+        <v>224</v>
+      </c>
+      <c r="G7" s="102" t="s">
+        <v>213</v>
+      </c>
+      <c r="H7" s="102" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="24" customHeight="1">
+      <c r="B8" s="98">
+        <f t="array" aca="1" ref="B8:H8" ca="1">INDEX(달력,ndx+2)</f>
+        <v>44144</v>
+      </c>
+      <c r="C8" s="98">
+        <f ca="1"/>
+        <v>44145</v>
+      </c>
+      <c r="D8" s="98">
+        <f ca="1"/>
+        <v>44146</v>
+      </c>
+      <c r="E8" s="98">
+        <f ca="1"/>
+        <v>44147</v>
+      </c>
+      <c r="F8" s="98">
+        <f ca="1"/>
+        <v>44148</v>
+      </c>
+      <c r="G8" s="100">
+        <f ca="1"/>
+        <v>44149</v>
+      </c>
+      <c r="H8" s="101">
+        <f ca="1"/>
+        <v>44150</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="51" customHeight="1">
+      <c r="B9" s="99" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="99" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="99" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="99" t="s">
+        <v>225</v>
+      </c>
+      <c r="F9" s="99" t="s">
+        <v>214</v>
+      </c>
+      <c r="G9" s="102" t="s">
+        <v>222</v>
+      </c>
+      <c r="H9" s="99"/>
+    </row>
+    <row r="10" spans="2:8" ht="24" customHeight="1">
+      <c r="B10" s="98">
+        <f t="array" aca="1" ref="B10:H10" ca="1">INDEX(달력,ndx+3)</f>
+        <v>44151</v>
+      </c>
+      <c r="C10" s="98">
+        <f ca="1"/>
+        <v>44152</v>
+      </c>
+      <c r="D10" s="98">
+        <f ca="1"/>
+        <v>44153</v>
+      </c>
+      <c r="E10" s="98">
+        <f ca="1"/>
+        <v>44154</v>
+      </c>
+      <c r="F10" s="98">
+        <f ca="1"/>
+        <v>44155</v>
+      </c>
+      <c r="G10" s="100">
+        <f ca="1"/>
+        <v>44156</v>
+      </c>
+      <c r="H10" s="101">
+        <f ca="1"/>
+        <v>44157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="51" customHeight="1">
+      <c r="B11" s="102" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+    </row>
+    <row r="12" spans="2:8" ht="24" customHeight="1">
+      <c r="B12" s="98">
+        <f t="array" aca="1" ref="B12:H12" ca="1">INDEX(달력,ndx+4)</f>
+        <v>44158</v>
+      </c>
+      <c r="C12" s="98">
+        <f ca="1"/>
+        <v>44159</v>
+      </c>
+      <c r="D12" s="98">
+        <f ca="1"/>
+        <v>44160</v>
+      </c>
+      <c r="E12" s="98">
+        <f ca="1"/>
+        <v>44161</v>
+      </c>
+      <c r="F12" s="98">
+        <f ca="1"/>
+        <v>44162</v>
+      </c>
+      <c r="G12" s="100">
+        <f ca="1"/>
+        <v>44163</v>
+      </c>
+      <c r="H12" s="101">
+        <f ca="1"/>
+        <v>44164</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="51" customHeight="1">
+      <c r="B13" s="99"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="99"/>
+    </row>
+    <row r="14" spans="2:8" ht="23.25" customHeight="1">
+      <c r="B14" s="98">
+        <f t="array" aca="1" ref="B14:H14" ca="1">INDEX(달력,ndx+5)</f>
+        <v>44165</v>
+      </c>
+      <c r="C14" s="98">
+        <f ca="1"/>
+        <v>44166</v>
+      </c>
+      <c r="D14" s="98">
+        <f ca="1"/>
+        <v>44167</v>
+      </c>
+      <c r="E14" s="98">
+        <f ca="1"/>
+        <v>44168</v>
+      </c>
+      <c r="F14" s="98">
+        <f ca="1"/>
+        <v>44169</v>
+      </c>
+      <c r="G14" s="98">
+        <f ca="1"/>
+        <v>44170</v>
+      </c>
+      <c r="H14" s="98">
+        <f ca="1"/>
+        <v>44171</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="51" customHeight="1">
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B6:H6">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:H8">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B8)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:H10">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:H12">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:H14">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:H4">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 행에는 이 달력의 요일 이름이 표시됩니다. 이 셀에는 주의 시작 요일이 표시됩니다. 시작 요일을 변경하려면 셀 E1에서 새 요일을 입력하거나 선택합니다." sqref="B3" xr:uid="{261DC67E-BD6B-4F4F-B3F7-600DA657D39A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에는 바로 위의 머리글인 3행에 표시된 요일에 해당하는 시작 날짜가 표시됩니다. 이 셀의 숫자가 1이 아닌 경우 해당 날짜는 이전 달의 날짜가 됩니다. 4, 6, 8, 10, 12, 14행에 각 요일에 해당하는 날짜가 표시됩니다." sqref="B4" xr:uid="{28639A83-92A4-4162-B70B-3A20A754F878}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이번 달이 12행이나 14행에서 끝나는 경우 12행이나 14행에 다음 달의 날짜가 표시될 수 있습니다." sqref="B12" xr:uid="{76E0E0CD-8554-48E1-87B3-ED1FF8276E91}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 요일 이름만 이 일정에 적용됩니다. 다시 시도를 선택하고 요일 이름을 직접 입력하거나 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 주 시작 요일을 선택합니다. 요일 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 요일을 선택하고 ENTER 키를 누릅니다." sqref="E1" xr:uid="{50028BE5-BED6-4E9C-9EEF-4D20696C8CDD}">
+      <formula1>"월요일,화요일,수요일,목요일,금요일,토요일,일요일"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 월 이름만 이 일정에 적용됩니다. 월 이름을 직접 입력하거나 목록에서 하나를 선택합니다. 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 월을 선택합니다. 월 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 월을 선택하고 ENTER 키를 누릅니다." sqref="C1:D1" xr:uid="{CBE5B2AD-ED79-4331-81D8-A728F6D8059A}">
+      <formula1>"1월,2월,3월,4월,5월,6월,7월,8월,9월,10월,11월,12월"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 달력은 연도나 월에 관계없이 월이 하나인 달력입니다. C1에서 월을 선택하고 B1에 연도를 입력합니다. 달력의 시작 요일을 E1에서 선택합니다. 5, 7, 9, 11, 13, 15 행에 일일 메모를 입력합니다." sqref="A1" xr:uid="{6F2BF1DD-2832-4A65-A42B-2143B8C8045A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="달력의 연도를 입력합니다." sqref="B1" xr:uid="{D99B9906-C028-43EF-B785-0EA17BA6C696}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에 일일 메모를 입력합니다. 5, 7, 9, 11, 13, 15행에는 일별 메모를 입력할 수 있는 셀이 있습니다." sqref="B5" xr:uid="{0F08B0D1-1C89-42B6-947E-E95E96F3F11F}"/>
+  </dataValidations>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.45" right="0.45" top="0.4" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="87" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1">
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727D1B76-AFF4-4223-844E-7562534489ED}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update moving and book
</commit_message>
<xml_diff>
--- a/Temp/이사준비-20200605.xlsx
+++ b/Temp/이사준비-20200605.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\03_doc\01_doc\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\04_doc\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E8270A-FFEE-419B-A93A-3ACAA9196F02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="840" activeTab="7"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="이사짐센터 견적" sheetId="7" r:id="rId1"/>
@@ -20,7 +21,8 @@
     <sheet name="MoveToXi" sheetId="3" r:id="rId6"/>
     <sheet name="OCT" sheetId="9" r:id="rId7"/>
     <sheet name="NOV" sheetId="10" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId9"/>
+    <sheet name="NOV (2)" sheetId="11" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'이사짐 센터 견적시 물품'!$C$5:$F$5</definedName>
@@ -28,42 +30,59 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'자이 입주시'!$A$5:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'현대아파트 이사'!$A$5:$K$84</definedName>
     <definedName name="DayToStart" localSheetId="7">NOV!$E$1</definedName>
+    <definedName name="DayToStart" localSheetId="8">'NOV (2)'!$E$1</definedName>
     <definedName name="DayToStart">OCT!$E$1</definedName>
     <definedName name="MonthToDisplay" localSheetId="7">NOV!$C$1</definedName>
+    <definedName name="MonthToDisplay" localSheetId="8">'NOV (2)'!$C$1</definedName>
     <definedName name="MonthToDisplay" localSheetId="6">OCT!$C$1</definedName>
     <definedName name="MonthToDisplayNumber" localSheetId="7">MATCH(NOV!MonthToDisplay,NOV!월,0)</definedName>
+    <definedName name="MonthToDisplayNumber" localSheetId="8">MATCH('NOV (2)'!MonthToDisplay,'NOV (2)'!월,0)</definedName>
     <definedName name="MonthToDisplayNumber" localSheetId="6">MATCH(OCT!MonthToDisplay,월,0)</definedName>
     <definedName name="ndx" localSheetId="7">ROUNDUP(MATCH(2,1/FREQUENCY(DATE(NOV!표시할연도,NOV!MonthToDisplayNumber,1),NOV!달력))/7,0)</definedName>
+    <definedName name="ndx" localSheetId="8">ROUNDUP(MATCH(2,1/FREQUENCY(DATE('NOV (2)'!표시할연도,'NOV (2)'!MonthToDisplayNumber,1),'NOV (2)'!달력))/7,0)</definedName>
     <definedName name="ndx" localSheetId="6">ROUNDUP(MATCH(2,1/FREQUENCY(DATE(OCT!표시할연도,OCT!MonthToDisplayNumber,1),OCT!달력))/7,0)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="7">NOV!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">'NOV (2)'!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">OCT!$3:$3</definedName>
     <definedName name="weekdays_reversed" localSheetId="7">{"일요일","토요일","금요일","목요일","수요일","화요일","월요일"}</definedName>
+    <definedName name="weekdays_reversed" localSheetId="8">{"일요일","토요일","금요일","목요일","수요일","화요일","월요일"}</definedName>
     <definedName name="weekdays_reversed">{"일요일","토요일","금요일","목요일","수요일","화요일","월요일"}</definedName>
     <definedName name="날짜눈금" localSheetId="7">NOV!요일+NOV!주*7</definedName>
+    <definedName name="날짜눈금" localSheetId="8">'NOV (2)'!요일+'NOV (2)'!주*7</definedName>
     <definedName name="날짜눈금">요일+주*7</definedName>
     <definedName name="날짜패턴" localSheetId="7">{1,1,2,2,3,3,4,4,5,5,6,6,7}</definedName>
+    <definedName name="날짜패턴" localSheetId="8">{1,1,2,2,3,3,4,4,5,5,6,6,7}</definedName>
     <definedName name="날짜패턴">{1,1,2,2,3,3,4,4,5,5,6,6,7}</definedName>
     <definedName name="달력" localSheetId="7">NOV!날짜눈금+NOV!첫째날짜-WEEKDAY(NOV!첫째날짜)-NOV!요일_옵션</definedName>
+    <definedName name="달력" localSheetId="8">'NOV (2)'!날짜눈금+'NOV (2)'!첫째날짜-WEEKDAY('NOV (2)'!첫째날짜)-'NOV (2)'!요일_옵션</definedName>
     <definedName name="달력" localSheetId="6">날짜눈금+OCT!첫째날짜-WEEKDAY(OCT!첫째날짜)-요일_옵션</definedName>
     <definedName name="시작날짜" localSheetId="7">DATE(NOV!표시할연도,NOV!월,1)</definedName>
+    <definedName name="시작날짜" localSheetId="8">DATE('NOV (2)'!표시할연도,'NOV (2)'!월,1)</definedName>
     <definedName name="시작날짜" localSheetId="6">DATE(OCT!표시할연도,OCT!월,1)</definedName>
     <definedName name="요일" localSheetId="7">{0,1,2,3,4,5,6}</definedName>
+    <definedName name="요일" localSheetId="8">{0,1,2,3,4,5,6}</definedName>
     <definedName name="요일">{0,1,2,3,4,5,6}</definedName>
     <definedName name="요일_옵션" localSheetId="7">MATCH(NOV!DayToStart,NOV!weekdays_reversed,0)-2</definedName>
+    <definedName name="요일_옵션" localSheetId="8">MATCH('NOV (2)'!DayToStart,'NOV (2)'!weekdays_reversed,0)-2</definedName>
     <definedName name="요일_옵션">MATCH(DayToStart,weekdays_reversed,0)-2</definedName>
     <definedName name="월" localSheetId="7">MATCH(NOV!MonthToDisplay,NOV!월,0)</definedName>
+    <definedName name="월" localSheetId="8">MATCH('NOV (2)'!MonthToDisplay,'NOV (2)'!월,0)</definedName>
     <definedName name="월" localSheetId="6">MATCH(OCT!MonthToDisplay,NOV!월,0)</definedName>
     <definedName name="월">{"1월","2월","3월","4월","5월","6월","7월","8월","9월","10월","11월","12월"}</definedName>
     <definedName name="주" localSheetId="7">{0;1;2;3;4;5;6}</definedName>
+    <definedName name="주" localSheetId="8">{0;1;2;3;4;5;6}</definedName>
     <definedName name="주">{0;1;2;3;4;5;6}</definedName>
     <definedName name="첫째날짜" localSheetId="7">DATE(NOV!표시할연도,NOV!월,1)</definedName>
+    <definedName name="첫째날짜" localSheetId="8">DATE('NOV (2)'!표시할연도,'NOV (2)'!월,1)</definedName>
     <definedName name="첫째날짜" localSheetId="6">DATE(OCT!표시할연도,OCT!월,1)</definedName>
     <definedName name="평일" localSheetId="7">{"월요일","화요일","수요일","목요일","금요일","토요일","일요일"}</definedName>
+    <definedName name="평일" localSheetId="8">{"월요일","화요일","수요일","목요일","금요일","토요일","일요일"}</definedName>
     <definedName name="평일">{"월요일","화요일","수요일","목요일","금요일","토요일","일요일"}</definedName>
     <definedName name="표시할연도" localSheetId="7">NOV!$B$1</definedName>
+    <definedName name="표시할연도" localSheetId="8">'NOV (2)'!$B$1</definedName>
     <definedName name="표시할연도" localSheetId="6">OCT!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -78,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="243">
   <si>
     <t>현대아파트 이사 준비</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -914,17 +933,6 @@
     <t>입주청소</t>
   </si>
   <si>
-    <t>잔금
-LED 리폼 가능성 타진</t>
-  </si>
-  <si>
-    <t>천장 청소
-아버지 생신</t>
-  </si>
-  <si>
-    <t>탄성코트 전처리</t>
-  </si>
-  <si>
     <t>탄성코트 전처리 &amp; 환기</t>
   </si>
   <si>
@@ -972,10 +980,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>이사?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>베이킹, 환기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -988,23 +992,158 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>정전기포, 물티슈, 청소도구(밀대)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <r>
+      <t xml:space="preserve">11/10 베이킹, 환기
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Malgun Gothic"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서(9/25)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11/19
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Malgun Gothic"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서(10/5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11/29
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Malgun Gothic"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서 10/15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>11/9 MON
+베이킹, 환기</t>
+  </si>
+  <si>
+    <t>11/15 SUN
+10AM 이사</t>
+  </si>
+  <si>
+    <t>11/3 TUE
+탄성코트</t>
+  </si>
+  <si>
+    <t>11/5 THU
+줄눈</t>
+  </si>
+  <si>
+    <t>11/7 SAT
+입주청소</t>
+  </si>
+  <si>
+    <t>11/14 SAT
+워시타워
+식기세척기</t>
+  </si>
+  <si>
+    <t>11/16 MON
+인덕션</t>
+  </si>
+  <si>
+    <t>10/30 FRI
+잔금
+LED 리폼 가능성 타진</t>
+  </si>
+  <si>
+    <t>10/31 SAT
+천장 청소
+아버지 생신</t>
+  </si>
+  <si>
+    <t>10/24 SAT
+아쿠아 수리 의뢰
+청소 용품 구매</t>
+  </si>
+  <si>
+    <t xml:space="preserve">정전기포, 물티슈, 청소도구(밀대), 라텍스장갑, 걸레, </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">새집증후군제거 - 베이크아웃, 야자활성탄(10kg) or 화목한가정, 공기청정기, 열교환기, 환기, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Malgun Gothic"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알델리트</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="aaaa"/>
-    <numFmt numFmtId="177" formatCode="dd"/>
+    <numFmt numFmtId="164" formatCode="aaaa"/>
+    <numFmt numFmtId="165" formatCode="dd"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1012,14 +1151,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1027,7 +1166,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1035,7 +1174,7 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1043,7 +1182,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1140,8 +1279,20 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Malgun Gothic"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Malgun Gothic"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1175,6 +1326,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1295,17 +1452,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="5" applyFill="0" applyProtection="0">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" applyFill="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="6" applyFill="0" applyProtection="0">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" applyFill="0" applyProtection="0">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1531,25 +1688,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="5" xfId="7" applyFont="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="7" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="5" xfId="7" applyFont="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="7" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="5" xfId="7" applyFont="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="5" xfId="7" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="6" xfId="8" applyFont="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="6" xfId="8" applyFont="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="9" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="6" xfId="8" applyFont="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="6" xfId="8" applyFont="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="6" xfId="8" applyFont="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="6" xfId="8" applyFont="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="7" xfId="9" applyFont="1" applyFill="1">
@@ -1558,6 +1715,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="9" applyFont="1" applyFill="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" xfId="9" applyFont="1" applyFill="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1620,18 +1783,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="날짜 설명" xfId="9"/>
-    <cellStyle name="오른쪽 정렬된 입력 레이블" xfId="6"/>
-    <cellStyle name="왼쪽 정렬된 입력 레이블" xfId="5"/>
-    <cellStyle name="제목 1 2" xfId="1"/>
-    <cellStyle name="제목 2 2" xfId="3"/>
-    <cellStyle name="제목 3 2" xfId="7"/>
-    <cellStyle name="제목 4 2" xfId="8"/>
-    <cellStyle name="제목 5" xfId="2"/>
+    <cellStyle name="날짜 설명" xfId="9" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="오른쪽 정렬된 입력 레이블" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="왼쪽 정렬된 입력 레이블" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="제목 1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="제목 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="제목 3 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="제목 4 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="제목 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="4"/>
+    <cellStyle name="표준 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1694,6 +1887,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1781,6 +1979,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1816,6 +2031,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1991,7 +2223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1999,22 +2231,22 @@
       <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.25" customWidth="1"/>
-    <col min="2" max="2" width="18.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="23.125" customWidth="1"/>
-    <col min="9" max="9" width="15.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="11" width="1.25" style="39" customWidth="1"/>
+    <col min="11" max="11" width="1.28515625" style="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" s="14" customFormat="1" ht="31.5">
+    <row r="1" spans="2:11" s="14" customFormat="1" ht="26.25">
       <c r="B1" s="14" t="s">
         <v>196</v>
       </c>
@@ -2038,29 +2270,29 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="2:11" s="1" customFormat="1">
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="88" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="84" t="s">
+      <c r="D5" s="90"/>
+      <c r="E5" s="86" t="s">
         <v>200</v>
       </c>
-      <c r="F5" s="84"/>
-      <c r="G5" s="85" t="s">
+      <c r="F5" s="86"/>
+      <c r="G5" s="87" t="s">
         <v>199</v>
       </c>
-      <c r="H5" s="85"/>
-      <c r="I5" s="84" t="s">
+      <c r="H5" s="87"/>
+      <c r="I5" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="J5" s="84"/>
+      <c r="J5" s="86"/>
       <c r="K5" s="38"/>
     </row>
     <row r="6" spans="2:11" s="1" customFormat="1">
-      <c r="B6" s="87"/>
+      <c r="B6" s="89"/>
       <c r="C6" s="33" t="s">
         <v>170</v>
       </c>
@@ -2213,7 +2445,7 @@
       </c>
       <c r="K11" s="37"/>
     </row>
-    <row r="12" spans="2:11" ht="33">
+    <row r="12" spans="2:11" ht="30">
       <c r="B12" s="34" t="s">
         <v>162</v>
       </c>
@@ -2370,7 +2602,7 @@
       <c r="J17" s="46"/>
       <c r="K17" s="37"/>
     </row>
-    <row r="18" spans="2:11" ht="49.5">
+    <row r="18" spans="2:11" ht="60">
       <c r="B18" s="13" t="s">
         <v>169</v>
       </c>
@@ -2426,7 +2658,7 @@
       <c r="J19" s="47"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="2:11" ht="33">
+    <row r="20" spans="2:11" ht="30">
       <c r="B20" s="34" t="s">
         <v>174</v>
       </c>
@@ -2574,7 +2806,7 @@
       <c r="K30" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:K5">
+  <autoFilter ref="B5:K5" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="3" showButton="0"/>
     <filterColumn colId="5" showButton="0"/>
@@ -2593,8 +2825,21 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G96"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2604,18 +2849,18 @@
       <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.25" customWidth="1"/>
-    <col min="2" max="2" width="13.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.75" customWidth="1"/>
-    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="1.25" style="39" customWidth="1"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="1.28515625" style="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="14" customFormat="1" ht="31.5">
+    <row r="1" spans="2:7" s="14" customFormat="1" ht="26.25">
       <c r="B1" s="15"/>
       <c r="C1" s="14" t="s">
         <v>0</v>
@@ -2654,10 +2899,10 @@
       <c r="G5" s="38"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="94" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="34" t="s">
@@ -2670,8 +2915,8 @@
       <c r="G6" s="32"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="95"/>
-      <c r="C7" s="92"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="94"/>
       <c r="D7" s="36" t="s">
         <v>25</v>
       </c>
@@ -2684,8 +2929,8 @@
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="95"/>
-      <c r="C8" s="96" t="s">
+      <c r="B8" s="97"/>
+      <c r="C8" s="98" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="36" t="s">
@@ -2698,8 +2943,8 @@
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="95"/>
-      <c r="C9" s="96"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="98"/>
       <c r="D9" s="34" t="s">
         <v>34</v>
       </c>
@@ -2710,8 +2955,8 @@
       <c r="G9" s="32"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="95"/>
-      <c r="C10" s="92" t="s">
+      <c r="B10" s="97"/>
+      <c r="C10" s="94" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="36" t="s">
@@ -2724,8 +2969,8 @@
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="95"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="94"/>
       <c r="D11" s="36" t="s">
         <v>114</v>
       </c>
@@ -2736,8 +2981,8 @@
       <c r="G11" s="37"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="95"/>
-      <c r="C12" s="92" t="s">
+      <c r="B12" s="97"/>
+      <c r="C12" s="94" t="s">
         <v>80</v>
       </c>
       <c r="D12" s="36" t="s">
@@ -2750,8 +2995,8 @@
       <c r="G12" s="32"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="95"/>
-      <c r="C13" s="92"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="94"/>
       <c r="D13" s="36" t="s">
         <v>84</v>
       </c>
@@ -2762,8 +3007,8 @@
       <c r="G13" s="37"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="95"/>
-      <c r="C14" s="92"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="36" t="s">
         <v>88</v>
       </c>
@@ -2774,8 +3019,8 @@
       <c r="G14" s="37"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="95"/>
-      <c r="C15" s="92"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="94"/>
       <c r="D15" s="36" t="s">
         <v>115</v>
       </c>
@@ -2802,7 +3047,7 @@
       <c r="G16" s="32"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="97" t="s">
         <v>147</v>
       </c>
       <c r="C17" s="35" t="s">
@@ -2818,7 +3063,7 @@
       <c r="G17" s="32"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="95"/>
+      <c r="B18" s="97"/>
       <c r="C18" s="35" t="s">
         <v>64</v>
       </c>
@@ -2832,10 +3077,10 @@
       <c r="G18" s="32"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="92" t="s">
+      <c r="C19" s="94" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="36" t="s">
@@ -2848,8 +3093,8 @@
       <c r="G19" s="32"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="90"/>
-      <c r="C20" s="92"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="94"/>
       <c r="D20" s="36" t="s">
         <v>17</v>
       </c>
@@ -2860,8 +3105,8 @@
       <c r="G20" s="32"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="90"/>
-      <c r="C21" s="92" t="s">
+      <c r="B21" s="92"/>
+      <c r="C21" s="94" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="36" t="s">
@@ -2874,8 +3119,8 @@
       <c r="G21" s="32"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="90"/>
-      <c r="C22" s="92"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="94"/>
       <c r="D22" s="36" t="s">
         <v>112</v>
       </c>
@@ -2886,7 +3131,7 @@
       <c r="G22" s="37"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="90"/>
+      <c r="B23" s="92"/>
       <c r="C23" s="35" t="s">
         <v>63</v>
       </c>
@@ -2900,8 +3145,8 @@
       <c r="G23" s="32"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="90"/>
-      <c r="C24" s="93" t="s">
+      <c r="B24" s="92"/>
+      <c r="C24" s="95" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="36" t="s">
@@ -2914,8 +3159,8 @@
       <c r="G24" s="32"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="90"/>
-      <c r="C25" s="94"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="96"/>
       <c r="D25" s="36" t="s">
         <v>72</v>
       </c>
@@ -2926,7 +3171,7 @@
       <c r="G25" s="32"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="90"/>
+      <c r="B26" s="92"/>
       <c r="C26" s="35" t="s">
         <v>100</v>
       </c>
@@ -2940,8 +3185,8 @@
       <c r="G26" s="32"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="90"/>
-      <c r="C27" s="93" t="s">
+      <c r="B27" s="92"/>
+      <c r="C27" s="95" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="36" t="s">
@@ -2954,8 +3199,8 @@
       <c r="G27" s="32"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="90"/>
-      <c r="C28" s="94"/>
+      <c r="B28" s="92"/>
+      <c r="C28" s="96"/>
       <c r="D28" s="36" t="s">
         <v>12</v>
       </c>
@@ -2966,8 +3211,8 @@
       <c r="G28" s="32"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="90"/>
-      <c r="C29" s="93" t="s">
+      <c r="B29" s="92"/>
+      <c r="C29" s="95" t="s">
         <v>81</v>
       </c>
       <c r="D29" s="36" t="s">
@@ -2980,8 +3225,8 @@
       <c r="G29" s="32"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="91"/>
-      <c r="C30" s="94"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="96"/>
       <c r="D30" s="36" t="s">
         <v>83</v>
       </c>
@@ -3962,7 +4207,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C5:F5"/>
+  <autoFilter ref="C5:F5" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="12">
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B6:B15"/>
@@ -3984,7 +4229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:D37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3994,16 +4239,16 @@
       <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.125" customWidth="1"/>
-    <col min="2" max="2" width="14.75" style="24" customWidth="1"/>
-    <col min="3" max="3" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" customWidth="1"/>
-    <col min="5" max="5" width="1.125" customWidth="1"/>
+    <col min="1" max="1" width="1.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="1.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="14" customFormat="1" ht="31.5">
+    <row r="1" spans="2:4" s="14" customFormat="1" ht="26.25">
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
@@ -4026,7 +4271,7 @@
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="100" t="s">
         <v>128</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -4035,35 +4280,35 @@
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="97"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="97"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="97"/>
+      <c r="B9" s="99"/>
       <c r="C9" s="6" t="s">
         <v>112</v>
       </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="97"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="6" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="99" t="s">
         <v>127</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -4072,28 +4317,28 @@
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="97"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="26" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="97"/>
+      <c r="B13" s="99"/>
       <c r="C13" s="26" t="s">
         <v>85</v>
       </c>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="2:4" s="21" customFormat="1">
-      <c r="B14" s="97"/>
+      <c r="B14" s="99"/>
       <c r="C14" s="26" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="97"/>
+      <c r="B15" s="99"/>
       <c r="C15" s="68" t="s">
         <v>56</v>
       </c>
@@ -4102,7 +4347,7 @@
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="97"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="68" t="s">
         <v>57</v>
       </c>
@@ -4111,28 +4356,28 @@
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="97"/>
+      <c r="B17" s="99"/>
       <c r="C17" s="6" t="s">
         <v>83</v>
       </c>
       <c r="D17" s="6"/>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="97"/>
+      <c r="B18" s="99"/>
       <c r="C18" s="6" t="s">
         <v>120</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="97"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="101" t="s">
         <v>130</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -4141,56 +4386,56 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="100"/>
+      <c r="B21" s="102"/>
       <c r="C21" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="100"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="100"/>
+      <c r="B23" s="102"/>
       <c r="C23" s="68" t="s">
         <v>110</v>
       </c>
       <c r="D23" s="68"/>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="100"/>
+      <c r="B24" s="102"/>
       <c r="C24" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="100"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="100"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="100"/>
+      <c r="B27" s="102"/>
       <c r="C27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="100"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="6" t="s">
         <v>121</v>
       </c>
@@ -4199,7 +4444,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" s="21" customFormat="1">
-      <c r="B29" s="100"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="6" t="s">
         <v>41</v>
       </c>
@@ -4208,49 +4453,49 @@
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="100"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="100"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="100"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="100"/>
+      <c r="B33" s="102"/>
       <c r="C33" s="6" t="s">
         <v>131</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="100"/>
+      <c r="B34" s="102"/>
       <c r="C34" s="6" t="s">
         <v>78</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="100"/>
+      <c r="B35" s="102"/>
       <c r="C35" s="6" t="s">
         <v>124</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="101"/>
+      <c r="B36" s="103"/>
       <c r="C36" s="6" t="s">
         <v>122</v>
       </c>
@@ -4270,7 +4515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4280,15 +4525,15 @@
       <selection pane="bottomRight" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" customWidth="1"/>
-    <col min="4" max="11" width="8.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="11" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="14" customFormat="1" ht="31.5">
+    <row r="1" spans="1:11" s="14" customFormat="1" ht="26.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -5858,14 +6103,14 @@
       <c r="K84" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:K84"/>
+  <autoFilter ref="A5:K84" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5875,16 +6120,16 @@
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="8.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" ht="31.5">
+    <row r="1" spans="1:5" s="14" customFormat="1" ht="26.25">
       <c r="A1" s="14" t="s">
         <v>103</v>
       </c>
@@ -6445,21 +6690,21 @@
       <c r="E63" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:E5"/>
+  <autoFilter ref="A5:E5" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -6476,22 +6721,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="72" customWidth="1"/>
-    <col min="2" max="8" width="23.625" style="72" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="72"/>
+    <col min="1" max="1" width="2.5703125" style="72" customWidth="1"/>
+    <col min="2" max="8" width="23.5703125" style="72" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45" customHeight="1">
@@ -6499,10 +6744,10 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2020</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="104" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="102"/>
+      <c r="D1" s="104"/>
       <c r="E1" s="71" t="s">
         <v>204</v>
       </c>
@@ -6511,10 +6756,10 @@
       <c r="B2" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="103"/>
+      <c r="D2" s="105"/>
       <c r="E2" s="74" t="s">
         <v>207</v>
       </c>
@@ -6702,7 +6947,9 @@
       <c r="D11" s="79"/>
       <c r="E11" s="79"/>
       <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
+      <c r="G11" s="79" t="s">
+        <v>240</v>
+      </c>
       <c r="H11" s="79"/>
     </row>
     <row r="12" spans="2:8" ht="24" customHeight="1">
@@ -6741,14 +6988,12 @@
       <c r="D13" s="79"/>
       <c r="E13" s="79"/>
       <c r="F13" s="82" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="G13" s="79" t="s">
-        <v>213</v>
-      </c>
-      <c r="H13" s="79" t="s">
-        <v>214</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="H13" s="79"/>
     </row>
     <row r="14" spans="2:8" ht="23.25" customHeight="1">
       <c r="B14" s="78" t="e">
@@ -6791,32 +7036,37 @@
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="72" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="72" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="72" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="72" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="72" t="s">
-        <v>231</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="72" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="72" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="2:2">
@@ -6828,6 +7078,399 @@
       <c r="B28" s="72" t="s">
         <v>210</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B6:H6">
+    <cfRule type="expression" dxfId="17" priority="6">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:H8">
+    <cfRule type="expression" dxfId="16" priority="5">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B8)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:H10">
+    <cfRule type="expression" dxfId="15" priority="4">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:H12">
+    <cfRule type="expression" dxfId="14" priority="3">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:H14">
+    <cfRule type="expression" dxfId="13" priority="2">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:H4">
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>MonthToDisplayNumber&lt;&gt;MONTH(B4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 행에는 이 달력의 요일 이름이 표시됩니다. 이 셀에는 주의 시작 요일이 표시됩니다. 시작 요일을 변경하려면 셀 E1에서 새 요일을 입력하거나 선택합니다." sqref="B3" xr:uid="{00000000-0002-0000-0600-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에는 바로 위의 머리글인 3행에 표시된 요일에 해당하는 시작 날짜가 표시됩니다. 이 셀의 숫자가 1이 아닌 경우 해당 날짜는 이전 달의 날짜가 됩니다. 4, 6, 8, 10, 12, 14행에 각 요일에 해당하는 날짜가 표시됩니다." sqref="B4" xr:uid="{00000000-0002-0000-0600-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이번 달이 12행이나 14행에서 끝나는 경우 12행이나 14행에 다음 달의 날짜가 표시될 수 있습니다." sqref="B12" xr:uid="{00000000-0002-0000-0600-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에 일일 메모를 입력합니다. 5, 7, 9, 11, 13, 15행에는 일별 메모를 입력할 수 있는 셀이 있습니다." sqref="B5" xr:uid="{00000000-0002-0000-0600-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="달력의 연도를 입력합니다." sqref="B1" xr:uid="{00000000-0002-0000-0600-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 달력은 연도나 월에 관계없이 월이 하나인 달력입니다. C1에서 월을 선택하고 B1에 연도를 입력합니다. 달력의 시작 요일을 E1에서 선택합니다. 5, 7, 9, 11, 13, 15 행에 일일 메모를 입력합니다." sqref="A1" xr:uid="{00000000-0002-0000-0600-000005000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 월 이름만 이 일정에 적용됩니다. 월 이름을 직접 입력하거나 목록에서 하나를 선택합니다. 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 월을 선택합니다. 월 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 월을 선택하고 ENTER 키를 누릅니다." sqref="C1:D1" xr:uid="{00000000-0002-0000-0600-000006000000}">
+      <formula1>"1월,2월,3월,4월,5월,6월,7월,8월,9월,10월,11월,12월"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 요일 이름만 이 일정에 적용됩니다. 다시 시도를 선택하고 요일 이름을 직접 입력하거나 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 주 시작 요일을 선택합니다. 요일 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 요일을 선택하고 ENTER 키를 누릅니다." sqref="E1" xr:uid="{00000000-0002-0000-0600-000007000000}">
+      <formula1>"월요일,화요일,수요일,목요일,금요일,토요일,일요일"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.45" right="0.45" top="0.4" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="87" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1">
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <tabColor theme="4" tint="-0.499984740745262"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:H15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="2.5703125" style="72" customWidth="1"/>
+    <col min="2" max="8" width="23.5703125" style="72" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="72"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="45" customHeight="1">
+      <c r="B1" s="70">
+        <f ca="1">YEAR(TODAY())</f>
+        <v>2020</v>
+      </c>
+      <c r="C1" s="104" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="104"/>
+      <c r="E1" s="71" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="30" customHeight="1">
+      <c r="B2" s="73" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="105" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="105"/>
+      <c r="E2" s="74" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B3" s="75" t="e">
+        <f t="array" aca="1" ref="B3:H3" ca="1">달력</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C3" s="75" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D3" s="75" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E3" s="75" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F3" s="75" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G3" s="75" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="H3" s="75" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="24" customHeight="1">
+      <c r="B4" s="78" t="e">
+        <f t="array" aca="1" ref="B4:H4" ca="1">INDEX(달력,ndx+0)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C4" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D4" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E4" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F4" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G4" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="H4" s="81" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="51" customHeight="1">
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="24" customHeight="1">
+      <c r="B6" s="78" t="e">
+        <f t="array" aca="1" ref="B6:H6" ca="1">INDEX(달력,ndx+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C6" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D6" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E6" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F6" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G6" s="80" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="H6" s="81" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="51" customHeight="1">
+      <c r="B7" s="83"/>
+      <c r="C7" s="82" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="83" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>221</v>
+      </c>
+      <c r="G7" s="82" t="s">
+        <v>235</v>
+      </c>
+      <c r="H7" s="82" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="24" customHeight="1">
+      <c r="B8" s="78" t="e">
+        <f t="array" aca="1" ref="B8:H8" ca="1">INDEX(달력,ndx+2)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C8" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D8" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E8" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F8" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G8" s="80" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="H8" s="81" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="51" customHeight="1">
+      <c r="B9" s="79" t="s">
+        <v>231</v>
+      </c>
+      <c r="C9" s="79" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="79" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="82" t="s">
+        <v>236</v>
+      </c>
+      <c r="H9" s="85" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="24" customHeight="1">
+      <c r="B10" s="78" t="e">
+        <f t="array" aca="1" ref="B10:H10" ca="1">INDEX(달력,ndx+3)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C10" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D10" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E10" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F10" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G10" s="80" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="H10" s="81" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="51" customHeight="1">
+      <c r="B11" s="82" t="s">
+        <v>237</v>
+      </c>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+    </row>
+    <row r="12" spans="2:8" ht="24" customHeight="1">
+      <c r="B12" s="78" t="e">
+        <f t="array" aca="1" ref="B12:H12" ca="1">INDEX(달력,ndx+4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C12" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D12" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E12" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F12" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G12" s="80" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="H12" s="81" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="51" customHeight="1">
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+    </row>
+    <row r="14" spans="2:8" ht="23.25" customHeight="1">
+      <c r="B14" s="78" t="e">
+        <f t="array" aca="1" ref="B14:H14" ca="1">INDEX(달력,ndx+5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C14" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D14" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="E14" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="F14" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G14" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="H14" s="78" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="51" customHeight="1">
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6866,18 +7509,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 행에는 이 달력의 요일 이름이 표시됩니다. 이 셀에는 주의 시작 요일이 표시됩니다. 시작 요일을 변경하려면 셀 E1에서 새 요일을 입력하거나 선택합니다." sqref="B3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에는 바로 위의 머리글인 3행에 표시된 요일에 해당하는 시작 날짜가 표시됩니다. 이 셀의 숫자가 1이 아닌 경우 해당 날짜는 이전 달의 날짜가 됩니다. 4, 6, 8, 10, 12, 14행에 각 요일에 해당하는 날짜가 표시됩니다." sqref="B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이번 달이 12행이나 14행에서 끝나는 경우 12행이나 14행에 다음 달의 날짜가 표시될 수 있습니다." sqref="B12"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에 일일 메모를 입력합니다. 5, 7, 9, 11, 13, 15행에는 일별 메모를 입력할 수 있는 셀이 있습니다." sqref="B5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="달력의 연도를 입력합니다." sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 달력은 연도나 월에 관계없이 월이 하나인 달력입니다. C1에서 월을 선택하고 B1에 연도를 입력합니다. 달력의 시작 요일을 E1에서 선택합니다. 5, 7, 9, 11, 13, 15 행에 일일 메모를 입력합니다." sqref="A1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 월 이름만 이 일정에 적용됩니다. 월 이름을 직접 입력하거나 목록에서 하나를 선택합니다. 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 월을 선택합니다. 월 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 월을 선택하고 ENTER 키를 누릅니다." sqref="C1:D1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 행에는 이 달력의 요일 이름이 표시됩니다. 이 셀에는 주의 시작 요일이 표시됩니다. 시작 요일을 변경하려면 셀 E1에서 새 요일을 입력하거나 선택합니다." sqref="B3" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에는 바로 위의 머리글인 3행에 표시된 요일에 해당하는 시작 날짜가 표시됩니다. 이 셀의 숫자가 1이 아닌 경우 해당 날짜는 이전 달의 날짜가 됩니다. 4, 6, 8, 10, 12, 14행에 각 요일에 해당하는 날짜가 표시됩니다." sqref="B4" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이번 달이 12행이나 14행에서 끝나는 경우 12행이나 14행에 다음 달의 날짜가 표시될 수 있습니다." sqref="B12" xr:uid="{00000000-0002-0000-0700-000002000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 요일 이름만 이 일정에 적용됩니다. 다시 시도를 선택하고 요일 이름을 직접 입력하거나 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 주 시작 요일을 선택합니다. 요일 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 요일을 선택하고 ENTER 키를 누릅니다." sqref="E1" xr:uid="{00000000-0002-0000-0700-000003000000}">
+      <formula1>"월요일,화요일,수요일,목요일,금요일,토요일,일요일"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 월 이름만 이 일정에 적용됩니다. 월 이름을 직접 입력하거나 목록에서 하나를 선택합니다. 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 월을 선택합니다. 월 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 월을 선택하고 ENTER 키를 누릅니다." sqref="C1:D1" xr:uid="{00000000-0002-0000-0700-000004000000}">
       <formula1>"1월,2월,3월,4월,5월,6월,7월,8월,9월,10월,11월,12월"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 요일 이름만 이 일정에 적용됩니다. 다시 시도를 선택하고 요일 이름을 직접 입력하거나 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 주 시작 요일을 선택합니다. 요일 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 요일을 선택하고 ENTER 키를 누릅니다." sqref="E1">
-      <formula1>"월요일,화요일,수요일,목요일,금요일,토요일,일요일"</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 달력은 연도나 월에 관계없이 월이 하나인 달력입니다. C1에서 월을 선택하고 B1에 연도를 입력합니다. 달력의 시작 요일을 E1에서 선택합니다. 5, 7, 9, 11, 13, 15 행에 일일 메모를 입력합니다." sqref="A1" xr:uid="{00000000-0002-0000-0700-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="달력의 연도를 입력합니다." sqref="B1" xr:uid="{00000000-0002-0000-0700-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에 일일 메모를 입력합니다. 5, 7, 9, 11, 13, 15행에는 일별 메모를 입력할 수 있는 셀이 있습니다." sqref="B5" xr:uid="{00000000-0002-0000-0700-000007000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.4" bottom="0.5" header="0.3" footer="0.3"/>
@@ -6888,23 +7531,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD11B490-5908-4BE3-8828-E870D4A11256}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="72" customWidth="1"/>
-    <col min="2" max="8" width="23.625" style="72" customWidth="1"/>
-    <col min="9" max="16384" width="9.125" style="72"/>
+    <col min="1" max="1" width="2.5703125" style="72" customWidth="1"/>
+    <col min="2" max="8" width="23.5703125" style="72" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="72"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45" customHeight="1">
@@ -6912,22 +7555,22 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2020</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="104" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="102"/>
+      <c r="D1" s="104"/>
       <c r="E1" s="71" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="30" customHeight="1">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="84" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="103"/>
+      <c r="D2" s="105"/>
       <c r="E2" s="74" t="s">
         <v>207</v>
       </c>
@@ -7000,7 +7643,7 @@
       <c r="F5" s="79"/>
       <c r="G5" s="79"/>
       <c r="H5" s="79" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="24" customHeight="1">
@@ -7036,22 +7679,22 @@
     <row r="7" spans="2:8" ht="51" customHeight="1">
       <c r="B7" s="83"/>
       <c r="C7" s="82" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D7" s="83" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E7" s="82" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G7" s="82" t="s">
         <v>211</v>
       </c>
       <c r="H7" s="82" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="24" customHeight="1">
@@ -7086,22 +7729,22 @@
     </row>
     <row r="9" spans="2:8" ht="51" customHeight="1">
       <c r="B9" s="79" t="s">
-        <v>220</v>
-      </c>
-      <c r="C9" s="79" t="s">
-        <v>220</v>
+        <v>217</v>
+      </c>
+      <c r="C9" s="83" t="s">
+        <v>228</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E9" s="79" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G9" s="82" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H9" s="79"/>
     </row>
@@ -7137,11 +7780,13 @@
     </row>
     <row r="11" spans="2:8" ht="51" customHeight="1">
       <c r="B11" s="82" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C11" s="79"/>
       <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
+      <c r="E11" s="79" t="s">
+        <v>229</v>
+      </c>
       <c r="F11" s="79"/>
       <c r="G11" s="79"/>
       <c r="H11" s="79"/>
@@ -7183,7 +7828,9 @@
       <c r="E13" s="79"/>
       <c r="F13" s="79"/>
       <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
+      <c r="H13" s="79" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="23.25" customHeight="1">
       <c r="B14" s="78" t="e">
@@ -7229,7 +7876,6 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B6:H6">
     <cfRule type="expression" dxfId="5" priority="6">
       <formula>MonthToDisplayNumber&lt;&gt;MONTH(B6)</formula>
@@ -7261,18 +7907,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 행에는 이 달력의 요일 이름이 표시됩니다. 이 셀에는 주의 시작 요일이 표시됩니다. 시작 요일을 변경하려면 셀 E1에서 새 요일을 입력하거나 선택합니다." sqref="B3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에는 바로 위의 머리글인 3행에 표시된 요일에 해당하는 시작 날짜가 표시됩니다. 이 셀의 숫자가 1이 아닌 경우 해당 날짜는 이전 달의 날짜가 됩니다. 4, 6, 8, 10, 12, 14행에 각 요일에 해당하는 날짜가 표시됩니다." sqref="B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이번 달이 12행이나 14행에서 끝나는 경우 12행이나 14행에 다음 달의 날짜가 표시될 수 있습니다." sqref="B12"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 요일 이름만 이 일정에 적용됩니다. 다시 시도를 선택하고 요일 이름을 직접 입력하거나 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 주 시작 요일을 선택합니다. 요일 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 요일을 선택하고 ENTER 키를 누릅니다." sqref="E1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 행에는 이 달력의 요일 이름이 표시됩니다. 이 셀에는 주의 시작 요일이 표시됩니다. 시작 요일을 변경하려면 셀 E1에서 새 요일을 입력하거나 선택합니다." sqref="B3" xr:uid="{D8C335D1-0883-431E-A324-9A194F3CF312}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에는 바로 위의 머리글인 3행에 표시된 요일에 해당하는 시작 날짜가 표시됩니다. 이 셀의 숫자가 1이 아닌 경우 해당 날짜는 이전 달의 날짜가 됩니다. 4, 6, 8, 10, 12, 14행에 각 요일에 해당하는 날짜가 표시됩니다." sqref="B4" xr:uid="{DC417EDA-C569-442C-8AEF-F64EFC76304A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이번 달이 12행이나 14행에서 끝나는 경우 12행이나 14행에 다음 달의 날짜가 표시될 수 있습니다." sqref="B12" xr:uid="{779DCC84-5655-4B92-908C-A9BAC48223BA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에 일일 메모를 입력합니다. 5, 7, 9, 11, 13, 15행에는 일별 메모를 입력할 수 있는 셀이 있습니다." sqref="B5" xr:uid="{D66DFBB3-C718-4FFA-A671-DFDC72385F06}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="달력의 연도를 입력합니다." sqref="B1" xr:uid="{C4B1011E-BCBD-49FB-80CA-DDAE64DC67B9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 달력은 연도나 월에 관계없이 월이 하나인 달력입니다. C1에서 월을 선택하고 B1에 연도를 입력합니다. 달력의 시작 요일을 E1에서 선택합니다. 5, 7, 9, 11, 13, 15 행에 일일 메모를 입력합니다." sqref="A1" xr:uid="{F328E7D3-3FEE-4737-BC06-D6EFD2214109}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 월 이름만 이 일정에 적용됩니다. 월 이름을 직접 입력하거나 목록에서 하나를 선택합니다. 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 월을 선택합니다. 월 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 월을 선택하고 ENTER 키를 누릅니다." sqref="C1:D1" xr:uid="{3F7E78F1-A86F-4FE7-98D2-13578D8110C1}">
+      <formula1>"1월,2월,3월,4월,5월,6월,7월,8월,9월,10월,11월,12월"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 요일 이름만 이 일정에 적용됩니다. 다시 시도를 선택하고 요일 이름을 직접 입력하거나 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 주 시작 요일을 선택합니다. 요일 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 요일을 선택하고 ENTER 키를 누릅니다." sqref="E1" xr:uid="{462F9299-FA2B-414B-A6B5-82190305DFB0}">
       <formula1>"월요일,화요일,수요일,목요일,금요일,토요일,일요일"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="유효한 월 이름만 이 일정에 적용됩니다. 월 이름을 직접 입력하거나 목록에서 하나를 선택합니다. 다시 시도를 선택하고 ALT + 아래쪽 화살표를 누른 다음 목록에서 선택합니다. 취소를 선택하여 셀을 종료합니다." prompt="이 달력의 월을 선택합니다. 월 이름을 직접 입력하거나 ALT+아래쪽 화살표를 누른 다음 목록에서 월을 선택하고 ENTER 키를 누릅니다." sqref="C1:D1">
-      <formula1>"1월,2월,3월,4월,5월,6월,7월,8월,9월,10월,11월,12월"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 달력은 연도나 월에 관계없이 월이 하나인 달력입니다. C1에서 월을 선택하고 B1에 연도를 입력합니다. 달력의 시작 요일을 E1에서 선택합니다. 5, 7, 9, 11, 13, 15 행에 일일 메모를 입력합니다." sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="달력의 연도를 입력합니다." sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="이 셀에 일일 메모를 입력합니다. 5, 7, 9, 11, 13, 15행에는 일별 메모를 입력할 수 있는 셀이 있습니다." sqref="B5"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.4" bottom="0.5" header="0.3" footer="0.3"/>
@@ -7281,17 +7927,4 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update book and moving
</commit_message>
<xml_diff>
--- a/Temp/이사준비-20200605.xlsx
+++ b/Temp/이사준비-20200605.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\04_doc\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E8270A-FFEE-419B-A93A-3ACAA9196F02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403EB142-6E9D-4748-9A67-C97B5C2E4D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="244">
   <si>
     <t>현대아파트 이사 준비</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -952,10 +952,6 @@
     <t>베이킹, 환기</t>
   </si>
   <si>
-    <t>TV 무타공 알아보기 - 이사전</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>탄성코트</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -985,10 +981,6 @@
   </si>
   <si>
     <t>LED 케이스 타공 실측</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>베이크아웃 방법 찾기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1074,10 +1066,6 @@
 베이킹, 환기</t>
   </si>
   <si>
-    <t>11/15 SUN
-10AM 이사</t>
-  </si>
-  <si>
     <t>11/3 TUE
 탄성코트</t>
   </si>
@@ -1088,15 +1076,6 @@
   <si>
     <t>11/7 SAT
 입주청소</t>
-  </si>
-  <si>
-    <t>11/14 SAT
-워시타워
-식기세척기</t>
-  </si>
-  <si>
-    <t>11/16 MON
-인덕션</t>
   </si>
   <si>
     <t>10/30 FRI
@@ -1114,11 +1093,8 @@
 청소 용품 구매</t>
   </si>
   <si>
-    <t xml:space="preserve">정전기포, 물티슈, 청소도구(밀대), 라텍스장갑, 걸레, </t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">새집증후군제거 - 베이크아웃, 야자활성탄(10kg) or 화목한가정, 공기청정기, 열교환기, 환기, </t>
+      <t xml:space="preserve">새집증후군제거 - 베이크아웃(온도 올리는 방법), 야자활성탄(10kg) or 화목한가정, 공기청정기, 열교환기, 환기, </t>
     </r>
     <r>
       <rPr>
@@ -1129,6 +1105,34 @@
       </rPr>
       <t>알델리트</t>
     </r>
+  </si>
+  <si>
+    <t>천장 선 청소</t>
+  </si>
+  <si>
+    <t>11/16 MON
+인덕션
+베이킹 / 환기</t>
+  </si>
+  <si>
+    <t>베이킹/환기</t>
+  </si>
+  <si>
+    <t>11/15 SUN
+10AM 이사
+베이킹/환기</t>
+  </si>
+  <si>
+    <t>11/14 SAT
+워시타워
+식기세척기
+베이킹/환기</t>
+  </si>
+  <si>
+    <t xml:space="preserve">입주청소 - 정전기 청소포, 물티슈, 청소도구(밀대), 라텍스장갑, 걸레, </t>
+  </si>
+  <si>
+    <t>탄성코트 - 선 청소, 선반제거 미리 부탁,</t>
   </si>
 </sst>
 </file>
@@ -1736,6 +1740,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1745,19 +1758,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2899,10 +2903,10 @@
       <c r="G5" s="38"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="91" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="94" t="s">
+      <c r="C6" s="92" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="34" t="s">
@@ -2915,8 +2919,8 @@
       <c r="G6" s="32"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="97"/>
-      <c r="C7" s="94"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="92"/>
       <c r="D7" s="36" t="s">
         <v>25</v>
       </c>
@@ -2929,8 +2933,8 @@
       <c r="G7" s="37"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="97"/>
-      <c r="C8" s="98" t="s">
+      <c r="B8" s="91"/>
+      <c r="C8" s="93" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="36" t="s">
@@ -2943,8 +2947,8 @@
       <c r="G8" s="37"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="97"/>
-      <c r="C9" s="98"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="93"/>
       <c r="D9" s="34" t="s">
         <v>34</v>
       </c>
@@ -2955,8 +2959,8 @@
       <c r="G9" s="32"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="97"/>
-      <c r="C10" s="94" t="s">
+      <c r="B10" s="91"/>
+      <c r="C10" s="92" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="36" t="s">
@@ -2969,8 +2973,8 @@
       <c r="G10" s="37"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="97"/>
-      <c r="C11" s="94"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
       <c r="D11" s="36" t="s">
         <v>114</v>
       </c>
@@ -2981,8 +2985,8 @@
       <c r="G11" s="37"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="97"/>
-      <c r="C12" s="94" t="s">
+      <c r="B12" s="91"/>
+      <c r="C12" s="92" t="s">
         <v>80</v>
       </c>
       <c r="D12" s="36" t="s">
@@ -2995,8 +2999,8 @@
       <c r="G12" s="32"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="97"/>
-      <c r="C13" s="94"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="92"/>
       <c r="D13" s="36" t="s">
         <v>84</v>
       </c>
@@ -3007,8 +3011,8 @@
       <c r="G13" s="37"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="97"/>
-      <c r="C14" s="94"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="92"/>
       <c r="D14" s="36" t="s">
         <v>88</v>
       </c>
@@ -3019,8 +3023,8 @@
       <c r="G14" s="37"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="97"/>
-      <c r="C15" s="94"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="92"/>
       <c r="D15" s="36" t="s">
         <v>115</v>
       </c>
@@ -3047,7 +3051,7 @@
       <c r="G16" s="32"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="91" t="s">
         <v>147</v>
       </c>
       <c r="C17" s="35" t="s">
@@ -3063,7 +3067,7 @@
       <c r="G17" s="32"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="97"/>
+      <c r="B18" s="91"/>
       <c r="C18" s="35" t="s">
         <v>64</v>
       </c>
@@ -3077,10 +3081,10 @@
       <c r="G18" s="32"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="94" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="94" t="s">
+      <c r="C19" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="36" t="s">
@@ -3093,8 +3097,8 @@
       <c r="G19" s="32"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="92"/>
-      <c r="C20" s="94"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="92"/>
       <c r="D20" s="36" t="s">
         <v>17</v>
       </c>
@@ -3105,8 +3109,8 @@
       <c r="G20" s="32"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="92"/>
-      <c r="C21" s="94" t="s">
+      <c r="B21" s="95"/>
+      <c r="C21" s="92" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="36" t="s">
@@ -3119,8 +3123,8 @@
       <c r="G21" s="32"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="92"/>
-      <c r="C22" s="94"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="92"/>
       <c r="D22" s="36" t="s">
         <v>112</v>
       </c>
@@ -3131,7 +3135,7 @@
       <c r="G22" s="37"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="92"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="35" t="s">
         <v>63</v>
       </c>
@@ -3145,8 +3149,8 @@
       <c r="G23" s="32"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="92"/>
-      <c r="C24" s="95" t="s">
+      <c r="B24" s="95"/>
+      <c r="C24" s="97" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="36" t="s">
@@ -3159,8 +3163,8 @@
       <c r="G24" s="32"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="92"/>
-      <c r="C25" s="96"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="98"/>
       <c r="D25" s="36" t="s">
         <v>72</v>
       </c>
@@ -3171,7 +3175,7 @@
       <c r="G25" s="32"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="92"/>
+      <c r="B26" s="95"/>
       <c r="C26" s="35" t="s">
         <v>100</v>
       </c>
@@ -3185,8 +3189,8 @@
       <c r="G26" s="32"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="92"/>
-      <c r="C27" s="95" t="s">
+      <c r="B27" s="95"/>
+      <c r="C27" s="97" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="36" t="s">
@@ -3199,8 +3203,8 @@
       <c r="G27" s="32"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="92"/>
-      <c r="C28" s="96"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="98"/>
       <c r="D28" s="36" t="s">
         <v>12</v>
       </c>
@@ -3211,8 +3215,8 @@
       <c r="G28" s="32"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="92"/>
-      <c r="C29" s="95" t="s">
+      <c r="B29" s="95"/>
+      <c r="C29" s="97" t="s">
         <v>81</v>
       </c>
       <c r="D29" s="36" t="s">
@@ -3225,8 +3229,8 @@
       <c r="G29" s="32"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="93"/>
-      <c r="C30" s="96"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="98"/>
       <c r="D30" s="36" t="s">
         <v>83</v>
       </c>
@@ -4209,18 +4213,18 @@
   </sheetData>
   <autoFilter ref="C5:F5" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="12">
+    <mergeCell ref="B19:B30"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C27:C28"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B6:B15"/>
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B19:B30"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C27:C28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6728,8 +6732,8 @@
   </sheetPr>
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -6948,7 +6952,7 @@
       <c r="E11" s="79"/>
       <c r="F11" s="79"/>
       <c r="G11" s="79" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H11" s="79"/>
     </row>
@@ -6988,10 +6992,10 @@
       <c r="D13" s="79"/>
       <c r="E13" s="79"/>
       <c r="F13" s="82" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G13" s="79" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="H13" s="79"/>
     </row>
@@ -7034,39 +7038,39 @@
       <c r="G15" s="79"/>
       <c r="H15" s="79"/>
     </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="72" t="s">
+        <v>213</v>
+      </c>
+    </row>
     <row r="18" spans="2:2">
       <c r="B18" s="72" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="72" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="72" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="72" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="72" t="s">
-        <v>227</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="72" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="72" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="72" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="2:2">
@@ -7286,22 +7290,22 @@
     <row r="7" spans="2:8" ht="51" customHeight="1">
       <c r="B7" s="83"/>
       <c r="C7" s="82" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D7" s="83" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="82" t="s">
+        <v>231</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>220</v>
+      </c>
+      <c r="G7" s="82" t="s">
+        <v>232</v>
+      </c>
+      <c r="H7" s="82" t="s">
         <v>222</v>
-      </c>
-      <c r="E7" s="82" t="s">
-        <v>234</v>
-      </c>
-      <c r="F7" s="79" t="s">
-        <v>221</v>
-      </c>
-      <c r="G7" s="82" t="s">
-        <v>235</v>
-      </c>
-      <c r="H7" s="82" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="24" customHeight="1">
@@ -7336,21 +7340,21 @@
     </row>
     <row r="9" spans="2:8" ht="51" customHeight="1">
       <c r="B9" s="79" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C9" s="79" t="s">
         <v>217</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E9" s="79"/>
       <c r="F9" s="79"/>
       <c r="G9" s="82" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="H9" s="85" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="24" customHeight="1">
@@ -7385,9 +7389,11 @@
     </row>
     <row r="11" spans="2:8" ht="51" customHeight="1">
       <c r="B11" s="82" t="s">
-        <v>237</v>
-      </c>
-      <c r="C11" s="79"/>
+        <v>238</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>239</v>
+      </c>
       <c r="D11" s="79"/>
       <c r="E11" s="79"/>
       <c r="F11" s="79"/>
@@ -7679,22 +7685,22 @@
     <row r="7" spans="2:8" ht="51" customHeight="1">
       <c r="B7" s="83"/>
       <c r="C7" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="83" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="D7" s="83" t="s">
-        <v>221</v>
-      </c>
-      <c r="E7" s="82" t="s">
+      <c r="F7" s="79" t="s">
         <v>220</v>
-      </c>
-      <c r="F7" s="79" t="s">
-        <v>221</v>
       </c>
       <c r="G7" s="82" t="s">
         <v>211</v>
       </c>
       <c r="H7" s="82" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="24" customHeight="1">
@@ -7732,16 +7738,16 @@
         <v>217</v>
       </c>
       <c r="C9" s="83" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E9" s="79" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F9" s="79" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G9" s="82" t="s">
         <v>215</v>
@@ -7785,7 +7791,7 @@
       <c r="C11" s="79"/>
       <c r="D11" s="79"/>
       <c r="E11" s="79" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F11" s="79"/>
       <c r="G11" s="79"/>
@@ -7829,7 +7835,7 @@
       <c r="F13" s="79"/>
       <c r="G13" s="79"/>
       <c r="H13" s="79" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="23.25" customHeight="1">

</xml_diff>